<commit_message>
Update code for Add rule
</commit_message>
<xml_diff>
--- a/SourceFiles/Rules.xlsx
+++ b/SourceFiles/Rules.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>RuleName</t>
   </si>
@@ -26,10 +26,25 @@
     <t>MatchType</t>
   </si>
   <si>
+    <t>Rule1</t>
+  </si>
+  <si>
+    <t>GL, CC, PC, Reporting Id</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Rule2</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
     <t>Rule3</t>
   </si>
   <si>
-    <t/>
+    <t>ISIN, Period</t>
   </si>
 </sst>
 </file>
@@ -75,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -106,7 +121,35 @@
         <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>